<commit_message>
Agregado el conjunto de reglas de MA_Rules para los chequeos referentes al Management. En curso la ejecución de las reglas en los enlaces asociados.
</commit_message>
<xml_diff>
--- a/CheckerRules/Resources/Results.xlsx
+++ b/CheckerRules/Resources/Results.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\Visual Studio Projects - 2017\Projects\CheckerRules\CheckerRules\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5059531E-0CF3-4B27-A0CB-D3AF41903E66}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA1CE77C-2165-4D9E-B262-F81234F9585B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{2D0D2D96-6920-4967-898F-B8AEEFBE7A27}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{2D0D2D96-6920-4967-898F-B8AEEFBE7A27}"/>
   </bookViews>
   <sheets>
     <sheet name="HOME" sheetId="1" r:id="rId1"/>
     <sheet name="Not Placed" sheetId="2" r:id="rId2"/>
     <sheet name="Not Enclosed" sheetId="3" r:id="rId3"/>
     <sheet name="Redundant" sheetId="4" r:id="rId4"/>
-    <sheet name="Rule 4" sheetId="5" r:id="rId5"/>
+    <sheet name="Project Units" sheetId="5" r:id="rId5"/>
     <sheet name="Rule 5" sheetId="6" r:id="rId6"/>
     <sheet name="Rule 6" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>Checker Rules BBI Revit add-in</t>
   </si>
@@ -118,6 +118,81 @@
   </si>
   <si>
     <t>AREA</t>
+  </si>
+  <si>
+    <t>Rule check results (Project Units)</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Length (Units)</t>
+  </si>
+  <si>
+    <t>Length (Rounding)</t>
+  </si>
+  <si>
+    <t>Area (Units)</t>
+  </si>
+  <si>
+    <t>Area (Rounding)</t>
+  </si>
+  <si>
+    <t>Volume (Units)</t>
+  </si>
+  <si>
+    <t>Volume (Rounding)</t>
+  </si>
+  <si>
+    <t>Angle (Units)</t>
+  </si>
+  <si>
+    <t>Angle (Rounding)</t>
+  </si>
+  <si>
+    <t>Slope (Units)</t>
+  </si>
+  <si>
+    <t>Slope (Rounding)</t>
+  </si>
+  <si>
+    <t>Currency (Units)</t>
+  </si>
+  <si>
+    <t>Currency (Rounding)</t>
+  </si>
+  <si>
+    <t>Mass Density (Units)</t>
+  </si>
+  <si>
+    <t>Mass Density (Rounding)</t>
+  </si>
+  <si>
+    <t>Milimeters</t>
+  </si>
+  <si>
+    <t>0 decimal places</t>
+  </si>
+  <si>
+    <t>Square meters</t>
+  </si>
+  <si>
+    <t>2 decimal places</t>
+  </si>
+  <si>
+    <t>Cubic meters</t>
+  </si>
+  <si>
+    <t>2 decimal meters</t>
+  </si>
+  <si>
+    <t>Decimal degrees</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Kilograms per cubic meter</t>
   </si>
 </sst>
 </file>
@@ -233,10 +308,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -245,6 +316,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,6 +349,30 @@
     <tableColumn id="3" xr3:uid="{FF5EBDBC-3DCD-46A9-980D-699D8D4CF21A}" name="Level"/>
     <tableColumn id="4" xr3:uid="{4AF0AA5E-C37A-4FFB-825A-D11876B6B582}" name="Phase"/>
     <tableColumn id="5" xr3:uid="{6CE121AC-52EC-4A11-ABC2-6E937AF4BCBC}" name="File"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{95E51C9D-4A0E-4CDA-9DA6-AE3FAB0608C0}" name="Tabla2" displayName="Tabla2" ref="A3:O4" totalsRowShown="0">
+  <autoFilter ref="A3:O4" xr:uid="{35281371-7683-44AB-B35C-60D120FB7D81}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{37E709EC-8422-4E05-A8B3-E201F0950215}" name="Length (Units)"/>
+    <tableColumn id="2" xr3:uid="{189F306C-EAEC-4DB4-8C6F-6AFDE51BAEE4}" name="Length (Rounding)"/>
+    <tableColumn id="3" xr3:uid="{10F115DD-4269-40AC-A050-1F81A936B173}" name="Area (Units)"/>
+    <tableColumn id="4" xr3:uid="{94A126C7-DA49-492B-9B5E-53F7D6400B4D}" name="Area (Rounding)"/>
+    <tableColumn id="5" xr3:uid="{2D27D811-3D65-4DB1-9A72-EF00090E02AC}" name="Volume (Units)"/>
+    <tableColumn id="6" xr3:uid="{BE3E0361-2157-4E85-A5CD-EAA63DECE8A0}" name="Volume (Rounding)"/>
+    <tableColumn id="7" xr3:uid="{FDD08C6B-B36E-4211-A2A6-CE2DE5CA698A}" name="Angle (Units)"/>
+    <tableColumn id="8" xr3:uid="{ADA7D6AA-0804-4E8E-BCEC-496685583B72}" name="Angle (Rounding)"/>
+    <tableColumn id="9" xr3:uid="{2E4EA746-8507-416D-8D3B-26665E784589}" name="Slope (Units)"/>
+    <tableColumn id="10" xr3:uid="{F8028F2C-0962-4D65-A668-8B186B602B6C}" name="Slope (Rounding)"/>
+    <tableColumn id="11" xr3:uid="{455036D1-ECB3-42C3-B434-7881C53798DE}" name="Currency (Units)"/>
+    <tableColumn id="12" xr3:uid="{6C31E3D6-DB0B-4D81-A5DE-5243D689371A}" name="Currency (Rounding)"/>
+    <tableColumn id="13" xr3:uid="{C9E3DE07-42B0-4B0C-8EAB-BEC4F3BBEB60}" name="Mass Density (Units)"/>
+    <tableColumn id="14" xr3:uid="{F245EF6B-E4BA-4602-BB15-9BA4953EEAA0}" name="Mass Density (Rounding)"/>
+    <tableColumn id="15" xr3:uid="{E83D8EB7-32D8-4EF0-9E6A-B3349C48F4D6}" name="File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -587,92 +688,92 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <v>44597.416666666664</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="4">
         <v>44597.446527777778</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>2.9861111111111113E-2</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="8"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
         <v>5</v>
       </c>
     </row>
@@ -691,8 +792,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -702,9 +803,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -787,6 +893,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -829,13 +938,152 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:O3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="25" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>